<commit_message>
show area for tornado coverage
</commit_message>
<xml_diff>
--- a/Results/20221006 sample4_subproblem_comparison.xlsx
+++ b/Results/20221006 sample4_subproblem_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D82EF24-2862-4B34-8B9C-AE3824A36E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1B029-DC1B-41B6-9774-577F022E7FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original_subproblem" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
   <si>
     <t>Budget :</t>
   </si>
@@ -177,6 +177,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609143</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526F5E23-8F5C-EE11-CA2F-7487A9CC7C63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="0"/>
+          <a:ext cx="3657143" cy="2361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -488,35 +537,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19D55DF-21E0-41A8-A0B2-8768F3EBD55F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>30000000</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>3600.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>3600.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.36328125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,71 +671,71 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3549.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3549.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -602,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -610,8 +751,350 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>-94.561999999999998</v>
+      </c>
+      <c r="C12">
+        <v>37.042999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>-94.5</v>
+      </c>
+      <c r="C13">
+        <v>37.090000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>291450206011012</v>
+      </c>
+      <c r="B16">
+        <v>-94.555999999999997</v>
+      </c>
+      <c r="C16">
+        <v>37.045000000000002</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>29284</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16">
+        <v>585369</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>290970112004069</v>
+      </c>
+      <c r="B17">
+        <v>-94.552000000000007</v>
+      </c>
+      <c r="C17">
+        <v>37.093000000000004</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>290970109002051</v>
+      </c>
+      <c r="B18">
+        <v>-94.551000000000002</v>
+      </c>
+      <c r="C18">
+        <v>37.058</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>59534</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <v>298961</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>290970110005024</v>
+      </c>
+      <c r="B19">
+        <v>-94.522000000000006</v>
+      </c>
+      <c r="C19">
+        <v>37.079000000000001</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <v>5637</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19">
+        <v>285809</v>
+      </c>
+      <c r="I19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>290970108003014</v>
+      </c>
+      <c r="B20">
+        <v>-94.516000000000005</v>
+      </c>
+      <c r="C20">
+        <v>37.07</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20">
+        <v>8484</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <v>306347</v>
+      </c>
+      <c r="I20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>290970101001022</v>
+      </c>
+      <c r="B21">
+        <v>-94.507000000000005</v>
+      </c>
+      <c r="C21">
+        <v>37.091999999999999</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>6959</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21">
+        <v>174902</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>290970106004001</v>
+      </c>
+      <c r="B22">
+        <v>-94.506</v>
+      </c>
+      <c r="C22">
+        <v>37.073999999999998</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>7311</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>290970106003025</v>
+      </c>
+      <c r="B23">
+        <v>-94.498000000000005</v>
+      </c>
+      <c r="C23">
+        <v>37.07</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23">
+        <v>17333</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>290970102001050</v>
+      </c>
+      <c r="B24">
+        <v>-94.474000000000004</v>
+      </c>
+      <c r="C24">
+        <v>37.113</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>290970104003071</v>
+      </c>
+      <c r="B25">
+        <v>-94.457999999999998</v>
+      </c>
+      <c r="C25">
+        <v>37.064999999999998</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>20376</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -620,7 +1103,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1.04</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -684,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.94</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -700,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.69</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -708,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -716,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>